<commit_message>
Send status added, general testing
</commit_message>
<xml_diff>
--- a/App/data/company_data.xlsx
+++ b/App/data/company_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Company_email</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Send_status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,9 @@
           <t>malas12x09@gmail.com</t>
         </is>
       </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +476,9 @@
           <t>yiceto2944@cpaurl.com</t>
         </is>
       </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -479,6 +490,9 @@
         <is>
           <t>mm@gmail.com</t>
         </is>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>